<commit_message>
Calcule la forecast error variance
</commit_message>
<xml_diff>
--- a/results/BIC_Models.xlsx
+++ b/results/BIC_Models.xlsx
@@ -17,10 +17,10 @@
     <t xml:space="preserve">results/c("ARMA(2,0)", "ARMA(0,1)", "ARMA(1,1)", "ARMA(2,1)", "ARMA(1,0)")</t>
   </si>
   <si>
-    <t xml:space="preserve">results/c(-53.1, -53, -50.2, -50.2, -35)</t>
+    <t xml:space="preserve">results/c(-54.4, -54.3, -51.5, -51.4, -36.3)</t>
   </si>
   <si>
-    <t xml:space="preserve">results/c(-63.3, -60.7, -60.4, -63, -42.7)</t>
+    <t xml:space="preserve">results/c(-64.7, -62, -61.8, -64.3, -44)</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fige l'IPI et finalise le projet
</commit_message>
<xml_diff>
--- a/results/BIC_Models.xlsx
+++ b/results/BIC_Models.xlsx
@@ -12,15 +12,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">results/c("ARMA(2,0)", "ARMA(0,1)", "ARMA(1,1)", "ARMA(2,1)", "ARMA(1,0)")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results/c(-54.4, -54.3, -51.5, -51.4, -36.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">results/c(-64.7, -62, -61.8, -64.3, -44)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t xml:space="preserve">Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMA(2,0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMA(0,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMA(1,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMA(2,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARMA(1,0)</t>
   </si>
 </sst>
 </file>
@@ -354,7 +369,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-54.4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-64.7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-54.3</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-62</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-51.5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-61.8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-51.4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-64.3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-36.3</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>